<commit_message>
Updated Resume and Credits
</commit_message>
<xml_diff>
--- a/resources/Credits.xlsx
+++ b/resources/Credits.xlsx
@@ -899,7 +899,7 @@
   <dimension ref="A2:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1917,7 +1917,7 @@
       <c r="B37" t="s">
         <v>133</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D37">
@@ -1954,7 +1954,7 @@
       <c r="B38" t="s">
         <v>133</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>125</v>
       </c>
       <c r="D38">
@@ -1991,7 +1991,7 @@
       <c r="B39" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D39">
@@ -2019,7 +2019,7 @@
       <c r="B40" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>107</v>
       </c>
       <c r="D40">
@@ -2047,7 +2047,7 @@
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="2" t="s">
         <v>140</v>
       </c>
       <c r="D41">
@@ -2078,7 +2078,7 @@
       <c r="A42" t="s">
         <v>109</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>123</v>
       </c>
       <c r="D42">
@@ -2109,7 +2109,7 @@
       </c>
     </row>
     <row r="43" spans="1:13">
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D43">
@@ -2134,7 +2134,7 @@
       <c r="A44" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="2" t="s">
         <v>143</v>
       </c>
       <c r="D44">
@@ -2156,7 +2156,7 @@
       </c>
     </row>
     <row r="45" spans="1:13">
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="2" t="s">
         <v>120</v>
       </c>
       <c r="D45">

</xml_diff>

<commit_message>
GreyHat Cryptography Presentation and Schedule Upate
</commit_message>
<xml_diff>
--- a/resources/Credits.xlsx
+++ b/resources/Credits.xlsx
@@ -589,7 +589,56 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -901,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2160,7 +2209,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C45" s="2" t="s">
-        <v>120</v>
+        <v>24</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -2169,14 +2218,17 @@
         <v>122</v>
       </c>
       <c r="F45" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="G45">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H45" t="s">
         <v>79</v>
       </c>
+      <c r="I45" t="s">
+        <v>88</v>
+      </c>
       <c r="L45">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2188,25 +2240,22 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C46" s="4" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E46" t="s">
         <v>124</v>
       </c>
       <c r="F46" t="s">
-        <v>99</v>
+        <v>23</v>
+      </c>
+      <c r="G46">
+        <v>4</v>
       </c>
       <c r="H46" t="s">
-        <v>78</v>
-      </c>
-      <c r="I46" t="s">
-        <v>91</v>
-      </c>
-      <c r="K46" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="L46">
         <f t="shared" si="0"/>
@@ -2219,22 +2268,25 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C47" s="4" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="D47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" t="s">
         <v>124</v>
       </c>
       <c r="F47" t="s">
-        <v>23</v>
-      </c>
-      <c r="G47">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="H47" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="I47" t="s">
+        <v>91</v>
+      </c>
+      <c r="K47" t="s">
+        <v>98</v>
       </c>
       <c r="L47">
         <f t="shared" si="0"/>
@@ -2247,7 +2299,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C48" s="4" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -2259,16 +2311,10 @@
         <v>23</v>
       </c>
       <c r="G48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H48" t="s">
-        <v>81</v>
-      </c>
-      <c r="I48" t="s">
-        <v>82</v>
-      </c>
-      <c r="J48" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="L48">
         <f t="shared" si="0"/>
@@ -2281,14 +2327,29 @@
     </row>
     <row r="49" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C49" s="4" t="s">
-        <v>149</v>
+        <v>22</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E49" t="s">
         <v>124</v>
       </c>
+      <c r="F49" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49" t="s">
+        <v>81</v>
+      </c>
+      <c r="I49" t="s">
+        <v>82</v>
+      </c>
+      <c r="J49" t="s">
+        <v>95</v>
+      </c>
       <c r="L49">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2300,25 +2361,13 @@
     </row>
     <row r="50" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C50" s="4" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
         <v>124</v>
-      </c>
-      <c r="F50" t="s">
-        <v>129</v>
-      </c>
-      <c r="G50">
-        <v>2</v>
-      </c>
-      <c r="H50" t="s">
-        <v>79</v>
-      </c>
-      <c r="I50" t="s">
-        <v>88</v>
       </c>
       <c r="L50">
         <f t="shared" si="0"/>
@@ -2473,8 +2522,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A7:K55">
-    <sortState ref="A8:K54">
-      <sortCondition ref="E7:E54"/>
+    <sortState ref="A8:K55">
+      <sortCondition sortBy="cellColor" ref="C7:C55" dxfId="1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated September List of GreyHat Presentations
</commit_message>
<xml_diff>
--- a/resources/Credits.xlsx
+++ b/resources/Credits.xlsx
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C48" s="4" t="s">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -2256,19 +2256,19 @@
         <v>123</v>
       </c>
       <c r="F48" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I48" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="J48" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="L48">
         <f t="shared" si="0"/>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="49" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C49" s="4" t="s">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="D49">
         <v>3</v>
@@ -2290,19 +2290,19 @@
         <v>123</v>
       </c>
       <c r="F49" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
       <c r="G49">
         <v>4</v>
       </c>
       <c r="H49" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I49" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J49" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="L49">
         <f t="shared" si="0"/>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="50" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C50" s="4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D50">
         <v>3</v>
@@ -2324,14 +2324,20 @@
         <v>140</v>
       </c>
       <c r="F50" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="G50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H50" t="s">
         <v>78</v>
       </c>
+      <c r="I50" t="s">
+        <v>126</v>
+      </c>
+      <c r="J50" t="s">
+        <v>95</v>
+      </c>
       <c r="L50">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2343,7 +2349,7 @@
     </row>
     <row r="51" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C51" s="4" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="D51">
         <v>3</v>
@@ -2352,19 +2358,13 @@
         <v>140</v>
       </c>
       <c r="F51" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G51">
         <v>4</v>
       </c>
       <c r="H51" t="s">
         <v>78</v>
-      </c>
-      <c r="I51" t="s">
-        <v>82</v>
-      </c>
-      <c r="J51" t="s">
-        <v>95</v>
       </c>
       <c r="L51">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Update Greyhat Presentations and Coursework
</commit_message>
<xml_diff>
--- a/resources/Credits.xlsx
+++ b/resources/Credits.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="150">
   <si>
     <t>Siddarth Senthilkumar</t>
   </si>
@@ -239,9 +239,6 @@
     <t>0 - Wellness</t>
   </si>
   <si>
-    <t>CS 4001 - Computing &amp; Society</t>
-  </si>
-  <si>
     <t>1 - Core A  - Essential Skills</t>
   </si>
   <si>
@@ -470,13 +467,16 @@
     <t>Options for extra credit hours: CS 8001 - Cybersecurity seminar, CS 4235 - Intro Info Security, Poetry, other CS classes</t>
   </si>
   <si>
-    <t>CS 6265 - Information Security Lab</t>
-  </si>
-  <si>
     <t>CETL 2000 - Undergraduate TA Prep</t>
   </si>
   <si>
     <t>CS 4699 - Undergraduate Research</t>
+  </si>
+  <si>
+    <t>CS 4235 - Intro. Information Security</t>
+  </si>
+  <si>
+    <t>CS 4002 - Robots &amp; Society</t>
   </si>
 </sst>
 </file>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,25 +922,25 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E4">
         <f>SUM(L8:L53) / SUM(M8:M53)</f>
-        <v>3.806451612903226</v>
+        <v>3.7972972972972974</v>
       </c>
       <c r="G4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -948,10 +948,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>62</v>
@@ -966,7 +966,7 @@
         <v>68</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>65</v>
@@ -978,18 +978,18 @@
         <v>67</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>44</v>
@@ -998,13 +998,13 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J8" t="s">
         <v>16</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
@@ -1032,10 +1032,10 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I9" t="s">
         <v>57</v>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>31</v>
@@ -1063,10 +1063,10 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I10" t="s">
         <v>56</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>35</v>
@@ -1094,10 +1094,10 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I11" t="s">
         <v>58</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>36</v>
@@ -1125,10 +1125,10 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I12" t="s">
         <v>58</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>42</v>
@@ -1156,16 +1156,16 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I13" t="s">
         <v>60</v>
       </c>
       <c r="J13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K13" t="s">
         <v>5</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>43</v>
@@ -1190,16 +1190,16 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I14" t="s">
         <v>24</v>
       </c>
       <c r="J14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K14" t="s">
         <v>6</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>32</v>
@@ -1224,10 +1224,10 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I15" t="s">
         <v>41</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>34</v>
@@ -1255,13 +1255,13 @@
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J16" t="s">
         <v>17</v>
@@ -1280,10 +1280,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>46</v>
@@ -1298,7 +1298,7 @@
         <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I17" t="s">
         <v>47</v>
@@ -1314,7 +1314,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>55</v>
@@ -1329,7 +1329,7 @@
         <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I18" t="s">
         <v>48</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>49</v>
@@ -1360,7 +1360,7 @@
         <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I19" t="s">
         <v>50</v>
@@ -1376,7 +1376,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>39</v>
@@ -1391,7 +1391,7 @@
         <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I20" t="s">
         <v>45</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>40</v>
@@ -1422,7 +1422,7 @@
         <v>5</v>
       </c>
       <c r="H21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I21" t="s">
         <v>59</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>29</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>52</v>
@@ -1487,7 +1487,7 @@
         <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I23" t="s">
         <v>51</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>53</v>
@@ -1518,7 +1518,7 @@
         <v>5</v>
       </c>
       <c r="H24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I24" t="s">
         <v>54</v>
@@ -1534,7 +1534,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>38</v>
@@ -1549,7 +1549,7 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I25" t="s">
         <v>61</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>37</v>
@@ -1580,7 +1580,7 @@
         <v>5</v>
       </c>
       <c r="H26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I26" t="s">
         <v>24</v>
@@ -1599,22 +1599,22 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27">
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G27">
         <v>5</v>
       </c>
       <c r="H27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L27">
         <f t="shared" si="0"/>
@@ -1627,13 +1627,13 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>18</v>
@@ -1670,10 +1670,10 @@
         <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L29">
         <f t="shared" si="0"/>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>19</v>
@@ -1701,10 +1701,10 @@
         <v>5</v>
       </c>
       <c r="H30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
@@ -1717,10 +1717,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1732,10 +1732,10 @@
         <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L31">
         <f t="shared" si="0"/>
@@ -1748,7 +1748,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>13</v>
@@ -1766,10 +1766,10 @@
         <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>20</v>
@@ -1791,7 +1791,7 @@
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F33" t="s">
         <v>21</v>
@@ -1800,10 +1800,10 @@
         <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L33">
         <f t="shared" si="0"/>
@@ -1816,28 +1816,28 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G34">
         <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L34">
         <f t="shared" si="0"/>
@@ -1850,25 +1850,25 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" t="s">
         <v>135</v>
-      </c>
-      <c r="D35">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F35" t="s">
-        <v>136</v>
       </c>
       <c r="G35">
         <v>5</v>
       </c>
       <c r="H35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>26</v>
@@ -1893,7 +1893,7 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F36" t="s">
         <v>27</v>
@@ -1902,7 +1902,7 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L36">
         <f t="shared" si="0"/>
@@ -1915,31 +1915,31 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D37">
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G37">
         <v>5</v>
       </c>
       <c r="H37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L37">
         <f t="shared" si="0"/>
@@ -1952,16 +1952,16 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
@@ -1970,13 +1970,13 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L38">
         <f t="shared" si="0"/>
@@ -1989,22 +1989,22 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G39">
         <v>5</v>
       </c>
       <c r="H39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L39">
         <f t="shared" si="0"/>
@@ -2017,25 +2017,25 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" t="s">
         <v>106</v>
-      </c>
-      <c r="D40">
-        <v>3</v>
-      </c>
-      <c r="E40" t="s">
-        <v>114</v>
-      </c>
-      <c r="F40" t="s">
-        <v>107</v>
       </c>
       <c r="G40">
         <v>5</v>
       </c>
       <c r="H40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L40">
         <f t="shared" si="0"/>
@@ -2047,42 +2047,48 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C41" s="2" t="s">
-        <v>149</v>
+      <c r="B41" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="E41" t="s">
+        <v>120</v>
+      </c>
+      <c r="F41" t="s">
+        <v>95</v>
+      </c>
+      <c r="H41" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" t="s">
+        <v>88</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F41" t="s">
-        <v>96</v>
-      </c>
-      <c r="H41" t="s">
-        <v>77</v>
-      </c>
-      <c r="I41" t="s">
-        <v>89</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C42" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="D42">
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F42" t="s">
         <v>22</v>
@@ -2091,60 +2097,66 @@
         <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M42">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C43" s="2" t="s">
-        <v>145</v>
+      <c r="B43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="D43">
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L43">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>148</v>
+        <v>107</v>
+      </c>
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L44">
         <f t="shared" si="0"/>
@@ -2156,85 +2168,94 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C45" s="2" t="s">
+      <c r="B45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D45">
         <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G45">
         <v>2</v>
       </c>
       <c r="H45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M45">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>122</v>
+      </c>
+      <c r="F46" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" t="s">
+        <v>76</v>
+      </c>
+      <c r="I46" t="s">
+        <v>89</v>
+      </c>
+      <c r="K46" t="s">
+        <v>96</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C47" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D46">
-        <v>3</v>
-      </c>
-      <c r="E46" t="s">
-        <v>123</v>
-      </c>
-      <c r="F46" t="s">
-        <v>98</v>
-      </c>
-      <c r="H46" t="s">
-        <v>77</v>
-      </c>
-      <c r="I46" t="s">
-        <v>90</v>
-      </c>
-      <c r="K46" t="s">
-        <v>97</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M46">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C47" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="D47">
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F47" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="G47">
         <v>4</v>
       </c>
       <c r="H47" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="I47" t="s">
+        <v>87</v>
+      </c>
+      <c r="J47" t="s">
+        <v>25</v>
       </c>
       <c r="L47">
         <f t="shared" si="0"/>
@@ -2246,29 +2267,29 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C48" s="4" t="s">
-        <v>70</v>
+      <c r="C48" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="D48">
         <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F48" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="G48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H48" t="s">
         <v>77</v>
       </c>
       <c r="I48" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="J48" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="L48">
         <f t="shared" si="0"/>
@@ -2280,29 +2301,23 @@
       </c>
     </row>
     <row r="49" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C49" s="4" t="s">
-        <v>138</v>
+      <c r="C49" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="D49">
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F49" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G49">
         <v>4</v>
       </c>
       <c r="H49" t="s">
-        <v>78</v>
-      </c>
-      <c r="I49" t="s">
-        <v>82</v>
-      </c>
-      <c r="J49" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="L49">
         <f t="shared" si="0"/>
@@ -2315,28 +2330,28 @@
     </row>
     <row r="50" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C50" s="4" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="D50">
         <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F50" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
       <c r="G50">
         <v>3</v>
       </c>
       <c r="H50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I50" t="s">
-        <v>126</v>
+        <v>81</v>
       </c>
       <c r="J50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L50">
         <f t="shared" si="0"/>
@@ -2349,22 +2364,22 @@
     </row>
     <row r="51" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C51" s="4" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="D51">
         <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F51" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H51" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L51">
         <f t="shared" si="0"/>
@@ -2377,13 +2392,22 @@
     </row>
     <row r="52" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C52" s="4" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="D52">
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="F52" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52">
+        <v>4</v>
+      </c>
+      <c r="H52" t="s">
+        <v>77</v>
       </c>
       <c r="L52">
         <f t="shared" si="0"/>
@@ -2396,25 +2420,25 @@
     </row>
     <row r="53" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C53" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D53">
         <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K53" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L53">
         <f t="shared" si="0"/>
@@ -2427,7 +2451,7 @@
     </row>
     <row r="54" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D54">
         <f>SUM(D8:D53)</f>

</xml_diff>

<commit_message>
Updated coursework and resume
Also added cookbook page!
</commit_message>
<xml_diff>
--- a/resources/Credits.xlsx
+++ b/resources/Credits.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Siddarth\Documents\GitHub\sidsenkumar11.github.io\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pikah\Documents\GitHub\sidsenkumar11.github.io\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$7:$K$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$7:$K$56</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="156">
   <si>
     <t>Siddarth Senthilkumar</t>
   </si>
@@ -113,9 +113,6 @@
     <t>MATH 2406</t>
   </si>
   <si>
-    <t>CS 3251</t>
-  </si>
-  <si>
     <t>APPH 1040 - Scientific Foundations of Health</t>
   </si>
   <si>
@@ -293,9 +290,6 @@
     <t>Computing/Robots in Society</t>
   </si>
   <si>
-    <t>Capstone - Project Design / Tech Comm Strategies</t>
-  </si>
-  <si>
     <t>Capstone - Project Implementation / Tech Comm Approaches</t>
   </si>
   <si>
@@ -401,9 +395,6 @@
     <t>ISYE 3770 - Intro. To Probability &amp; Statistics</t>
   </si>
   <si>
-    <t>CS 4210 - Advanced Operating Systems or CS 4290 - Advanced Computer Organization</t>
-  </si>
-  <si>
     <t>Advanced Systems &amp; Architectures</t>
   </si>
   <si>
@@ -440,9 +431,6 @@
     <t>HTS 2927 - What is Europe?</t>
   </si>
   <si>
-    <t>CS 4237 - Computer &amp; Network Security / ECE 4112 Internetwork Security /  ECE 4894 Intro to Computer Security / CS 4803 Special Topics CS 6265 Information Security Lab</t>
-  </si>
-  <si>
     <t>CETL 2001 - Fundamentals of Peer Tutoring</t>
   </si>
   <si>
@@ -464,9 +452,6 @@
     <t>CS 4903 - Undergraduate TA</t>
   </si>
   <si>
-    <t>Options for extra credit hours: CS 8001 - Cybersecurity seminar, CS 4235 - Intro Info Security, Poetry, other CS classes</t>
-  </si>
-  <si>
     <t>CETL 2000 - Undergraduate TA Prep</t>
   </si>
   <si>
@@ -477,13 +462,46 @@
   </si>
   <si>
     <t>CS 4002 - Robots &amp; Society</t>
+  </si>
+  <si>
+    <t>CS 3311 - Project Design</t>
+  </si>
+  <si>
+    <t>LMC 3432 - Tech Comm Strategies</t>
+  </si>
+  <si>
+    <t>CS 2340 and CS 3311</t>
+  </si>
+  <si>
+    <t>CS 4290 - Advanced Computer Organization</t>
+  </si>
+  <si>
+    <t>CS 3312 - Project Implementation</t>
+  </si>
+  <si>
+    <t>LMC 3431 - Tech Comm Approaches</t>
+  </si>
+  <si>
+    <t>CS 2340 and LMC 3431</t>
+  </si>
+  <si>
+    <t>CS 2340 and CS 3312</t>
+  </si>
+  <si>
+    <t>Options for extra credit hours: CS 8001 - Cybersecurity seminar, Poetry, other CS classes</t>
+  </si>
+  <si>
+    <t>Security Classes: CS 4237 - Computer &amp; Network Security / ECE 4112 Internetwork Security /  ECE 4894 Intro to Computer Security / CS 4803 Special Topics CS 6265 Information Security Lab</t>
+  </si>
+  <si>
+    <t>MGT 3078 - Finance &amp; Investments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,13 +524,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,7 +532,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,11 +547,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -562,25 +568,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -893,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M54"/>
+  <dimension ref="A2:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,89 +925,92 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E4">
-        <f>SUM(L8:L53) / SUM(M8:M53)</f>
-        <v>3.7972972972972974</v>
+        <f>SUM(L8:L55) / SUM(M8:M55)</f>
+        <v>3.8255813953488373</v>
       </c>
       <c r="G4" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>112</v>
+        <v>110</v>
+      </c>
+      <c r="G5" t="s">
+        <v>154</v>
       </c>
       <c r="L5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="A7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>143</v>
+      <c r="K7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J8" t="s">
         <v>16</v>
@@ -1023,53 +1029,53 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K9" t="s">
         <v>7</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L9:L53" si="0">IF(B9="T",0,IF(A9="Yes",0,IF(B9="S",0,IF(B9="", 0, (IF(B9="F", 0, IF(B9="D", 1, IF(B9="C", 2, IF(B9="B", 3, IF(B9="A", 4, 0)))))) * D9))))</f>
+        <f t="shared" ref="L9:L55" si="0">IF(B9="T",0,IF(A9="Yes",0,IF(B9="S",0,IF(B9="", 0, (IF(B9="F", 0, IF(B9="D", 1, IF(B9="C", 2, IF(B9="B", 3, IF(B9="A", 4, 0)))))) * D9))))</f>
         <v>0</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M9:M53" si="1">IF(B9="T",0,IF(A9="Yes",0,IF(B9="S",0,IF(B9="", 0, D9))))</f>
+        <f t="shared" ref="M9:M55" si="1">IF(B9="T",0,IF(A9="Yes",0,IF(B9="S",0,IF(B9="", 0, D9))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K10" t="s">
         <v>1</v>
@@ -1085,22 +1091,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K11" t="s">
         <v>11</v>
@@ -1116,22 +1122,22 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K12" t="s">
         <v>11</v>
@@ -1147,25 +1153,25 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K13" t="s">
         <v>5</v>
@@ -1181,25 +1187,25 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I14" t="s">
         <v>24</v>
       </c>
       <c r="J14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K14" t="s">
         <v>6</v>
@@ -1215,22 +1221,22 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K15" t="s">
         <v>3</v>
@@ -1246,22 +1252,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J16" t="s">
         <v>17</v>
@@ -1280,13 +1286,13 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1298,10 +1304,10 @@
         <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
@@ -1314,10 +1320,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1329,10 +1335,10 @@
         <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
@@ -1345,10 +1351,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -1360,10 +1366,10 @@
         <v>5</v>
       </c>
       <c r="H19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
@@ -1376,10 +1382,10 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -1391,10 +1397,10 @@
         <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L20">
         <f t="shared" si="0"/>
@@ -1407,10 +1413,10 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -1422,10 +1428,10 @@
         <v>5</v>
       </c>
       <c r="H21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J21" t="s">
         <v>9</v>
@@ -1441,10 +1447,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1456,10 +1462,10 @@
         <v>4</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L22">
         <f t="shared" si="0"/>
@@ -1472,10 +1478,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1487,10 +1493,10 @@
         <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
@@ -1503,10 +1509,10 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1518,10 +1524,10 @@
         <v>5</v>
       </c>
       <c r="H24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L24">
         <f t="shared" si="0"/>
@@ -1534,10 +1540,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25">
         <v>4</v>
@@ -1549,10 +1555,10 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
@@ -1565,10 +1571,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1580,7 +1586,7 @@
         <v>5</v>
       </c>
       <c r="H26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I26" t="s">
         <v>24</v>
@@ -1599,22 +1605,22 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D27">
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G27">
         <v>5</v>
       </c>
       <c r="H27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L27">
         <f t="shared" si="0"/>
@@ -1627,13 +1633,13 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1655,7 +1661,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>18</v>
@@ -1670,10 +1676,10 @@
         <v>3</v>
       </c>
       <c r="H29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L29">
         <f t="shared" si="0"/>
@@ -1686,7 +1692,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>19</v>
@@ -1701,10 +1707,10 @@
         <v>5</v>
       </c>
       <c r="H30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
@@ -1717,10 +1723,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1732,10 +1738,10 @@
         <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L31">
         <f t="shared" si="0"/>
@@ -1748,7 +1754,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>13</v>
@@ -1766,10 +1772,10 @@
         <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L32">
         <f t="shared" si="0"/>
@@ -1782,7 +1788,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>20</v>
@@ -1791,7 +1797,7 @@
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F33" t="s">
         <v>21</v>
@@ -1800,10 +1806,10 @@
         <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L33">
         <f t="shared" si="0"/>
@@ -1816,28 +1822,28 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G34">
         <v>2</v>
       </c>
       <c r="H34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L34">
         <f t="shared" si="0"/>
@@ -1850,25 +1856,25 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="D35">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G35">
         <v>5</v>
       </c>
       <c r="H35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L35">
         <f t="shared" si="0"/>
@@ -1881,10 +1887,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>26</v>
@@ -1893,7 +1899,7 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F36" t="s">
         <v>27</v>
@@ -1902,7 +1908,7 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L36">
         <f t="shared" si="0"/>
@@ -1915,31 +1921,31 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D37">
         <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F37" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G37">
         <v>5</v>
       </c>
       <c r="H37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L37">
         <f t="shared" si="0"/>
@@ -1952,16 +1958,16 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
@@ -1970,13 +1976,13 @@
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L38">
         <f t="shared" si="0"/>
@@ -1989,22 +1995,22 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G39">
         <v>5</v>
       </c>
       <c r="H39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L39">
         <f t="shared" si="0"/>
@@ -2017,25 +2023,25 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G40">
         <v>5</v>
       </c>
       <c r="H40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L40">
         <f t="shared" si="0"/>
@@ -2048,25 +2054,19 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>120</v>
-      </c>
-      <c r="F41" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="H41" t="s">
-        <v>76</v>
-      </c>
-      <c r="I41" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="L41">
         <f t="shared" si="0"/>
@@ -2079,16 +2079,16 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F42" t="s">
         <v>22</v>
@@ -2097,13 +2097,13 @@
         <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L42">
         <f t="shared" si="0"/>
@@ -2116,19 +2116,19 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D43">
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L43">
         <f t="shared" si="0"/>
@@ -2141,22 +2141,22 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L44">
         <f t="shared" si="0"/>
@@ -2169,7 +2169,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>23</v>
@@ -2178,19 +2178,19 @@
         <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F45" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G45">
         <v>2</v>
       </c>
       <c r="H45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L45">
         <f t="shared" si="0"/>
@@ -2202,184 +2202,205 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C46" s="2" t="s">
+      <c r="B46" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>120</v>
+      </c>
+      <c r="F46" t="s">
+        <v>95</v>
+      </c>
+      <c r="G46">
+        <v>5</v>
+      </c>
+      <c r="H46" t="s">
+        <v>75</v>
+      </c>
+      <c r="I46" t="s">
+        <v>87</v>
+      </c>
+      <c r="K46" t="s">
+        <v>94</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>120</v>
+      </c>
+      <c r="F47" t="s">
         <v>147</v>
       </c>
-      <c r="D46">
-        <v>3</v>
-      </c>
-      <c r="E46" t="s">
-        <v>122</v>
-      </c>
-      <c r="F46" t="s">
-        <v>97</v>
-      </c>
-      <c r="H46" t="s">
-        <v>76</v>
-      </c>
-      <c r="I46" t="s">
-        <v>89</v>
-      </c>
-      <c r="K46" t="s">
-        <v>96</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M46">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C47" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D47">
-        <v>3</v>
-      </c>
-      <c r="E47" t="s">
-        <v>122</v>
-      </c>
-      <c r="F47" t="s">
-        <v>116</v>
-      </c>
       <c r="G47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I47" t="s">
         <v>87</v>
       </c>
-      <c r="J47" t="s">
+      <c r="L47">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>120</v>
+      </c>
+      <c r="F48" t="s">
+        <v>114</v>
+      </c>
+      <c r="G48">
+        <v>4</v>
+      </c>
+      <c r="H48" t="s">
+        <v>75</v>
+      </c>
+      <c r="I48" t="s">
+        <v>86</v>
+      </c>
+      <c r="J48" t="s">
         <v>25</v>
       </c>
-      <c r="L47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M47">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C48" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D48">
-        <v>3</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="L48">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>120</v>
+      </c>
+      <c r="F49" t="s">
+        <v>123</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49" t="s">
+        <v>76</v>
+      </c>
+      <c r="I49" t="s">
         <v>122</v>
       </c>
-      <c r="F48" t="s">
-        <v>126</v>
-      </c>
-      <c r="G48">
-        <v>3</v>
-      </c>
-      <c r="H48" t="s">
-        <v>77</v>
-      </c>
-      <c r="I48" t="s">
-        <v>125</v>
-      </c>
-      <c r="J48" t="s">
-        <v>94</v>
-      </c>
-      <c r="L48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M48">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C49" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D49">
-        <v>3</v>
-      </c>
-      <c r="E49" t="s">
-        <v>122</v>
-      </c>
-      <c r="F49" t="s">
-        <v>22</v>
-      </c>
-      <c r="G49">
-        <v>4</v>
-      </c>
-      <c r="H49" t="s">
-        <v>77</v>
+      <c r="J49" t="s">
+        <v>92</v>
       </c>
       <c r="L49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M49">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C50" s="4" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="D50">
         <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="F50" t="s">
         <v>22</v>
       </c>
       <c r="G50">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H50" t="s">
-        <v>77</v>
-      </c>
-      <c r="I50" t="s">
-        <v>81</v>
-      </c>
-      <c r="J50" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="L50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M50">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C51" s="4" t="s">
-        <v>137</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C51" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="D51">
         <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F51" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G51">
         <v>3</v>
       </c>
       <c r="H51" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="I51" t="s">
+        <v>80</v>
+      </c>
+      <c r="J51" t="s">
+        <v>92</v>
       </c>
       <c r="L51">
         <f t="shared" si="0"/>
@@ -2390,56 +2411,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C52" s="4" t="s">
-        <v>118</v>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C52" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="D52">
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>139</v>
-      </c>
-      <c r="F52" t="s">
+        <v>135</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52" t="s">
+        <v>78</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C53" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>135</v>
+      </c>
+      <c r="F53" t="s">
         <v>22</v>
       </c>
-      <c r="G52">
-        <v>4</v>
-      </c>
-      <c r="H52" t="s">
-        <v>77</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C53" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D53">
-        <v>3</v>
-      </c>
-      <c r="E53" t="s">
-        <v>139</v>
-      </c>
-      <c r="F53" t="s">
-        <v>97</v>
+      <c r="G53">
+        <v>1</v>
       </c>
       <c r="H53" t="s">
         <v>76</v>
       </c>
-      <c r="I53" t="s">
-        <v>89</v>
-      </c>
-      <c r="K53" t="s">
-        <v>96</v>
-      </c>
       <c r="L53">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2449,17 +2464,82 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>101</v>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C54" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="D54">
-        <f>SUM(D8:D53)</f>
+        <v>2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>135</v>
+      </c>
+      <c r="F54" t="s">
+        <v>151</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+      <c r="H54" t="s">
+        <v>75</v>
+      </c>
+      <c r="I54" t="s">
+        <v>87</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C55" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>135</v>
+      </c>
+      <c r="F55" t="s">
+        <v>152</v>
+      </c>
+      <c r="G55">
+        <v>4</v>
+      </c>
+      <c r="H55" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" t="s">
+        <v>87</v>
+      </c>
+      <c r="K55" t="s">
+        <v>94</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56">
+        <f>SUM(D8:D55)</f>
         <v>137</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:K54">
+  <autoFilter ref="A7:K56">
     <sortState ref="A8:K54">
       <sortCondition ref="E7:E54"/>
     </sortState>

</xml_diff>

<commit_message>
Updated resume and courses
</commit_message>
<xml_diff>
--- a/resources/Credits.xlsx
+++ b/resources/Credits.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pikah\Documents\GitHub\sidsenkumar11.github.io\resources\"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="155">
   <si>
     <t>Siddarth Senthilkumar</t>
   </si>
@@ -492,9 +492,6 @@
   </si>
   <si>
     <t>Security Classes: CS 4237 - Computer &amp; Network Security / ECE 4112 Internetwork Security /  ECE 4894 Intro to Computer Security / CS 4803 Special Topics CS 6265 Information Security Lab</t>
-  </si>
-  <si>
-    <t>MGT 3078 - Finance &amp; Investments</t>
   </si>
 </sst>
 </file>
@@ -2413,7 +2410,7 @@
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D52">
         <v>3</v>

</xml_diff>